<commit_message>
add alert mail + bug a regler date flights list
</commit_message>
<xml_diff>
--- a/glproject/src/main/resources/flight list.xlsx
+++ b/glproject/src/main/resources/flight list.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="991" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Feuille1" sheetId="1" state="visible" r:id="rId2"/>
@@ -20,76 +20,84 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="18">
-  <si>
-    <t xml:space="preserve">idPlane</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">commercia</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">l</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">depAirport</t>
-  </si>
-  <si>
-    <t xml:space="preserve">arrAirport</t>
-  </si>
-  <si>
-    <t xml:space="preserve">depTime</t>
-  </si>
-  <si>
-    <t xml:space="preserve">arrTime</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TVA1234</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LFPA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LFPO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GVF1224</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AGPW</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TVT1234</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LPPO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MLPO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TVF1439</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PVI1234</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TSF1214</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LKPO</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="24">
+  <si>
+    <t>idPlane</t>
+  </si>
+  <si>
+    <t>commercial</t>
+  </si>
+  <si>
+    <t>depAirport</t>
+  </si>
+  <si>
+    <t>arrAirport</t>
+  </si>
+  <si>
+    <t>depTime</t>
+  </si>
+  <si>
+    <t>arrTime</t>
+  </si>
+  <si>
+    <t>TVA1234</t>
+  </si>
+  <si>
+    <t>LFPA</t>
+  </si>
+  <si>
+    <t>LFPO</t>
+  </si>
+  <si>
+    <t>01/01/2011 12:00
+</t>
+  </si>
+  <si>
+    <t>GVF1224</t>
+  </si>
+  <si>
+    <t>AGPW</t>
+  </si>
+  <si>
+    <t>02/01/2011 12:00
+</t>
+  </si>
+  <si>
+    <t>TVT1234</t>
+  </si>
+  <si>
+    <t>LPPO</t>
+  </si>
+  <si>
+    <t>MLPO</t>
+  </si>
+  <si>
+    <t>03/01/2011 12:00
+</t>
+  </si>
+  <si>
+    <t>TVF1439</t>
+  </si>
+  <si>
+    <t>04/01/2011 12:00
+</t>
+  </si>
+  <si>
+    <t>PVI1234</t>
+  </si>
+  <si>
+    <t>05/01/2011 12:00
+</t>
+  </si>
+  <si>
+    <t>TSF1214</t>
+  </si>
+  <si>
+    <t>LKPO</t>
+  </si>
+  <si>
+    <t>06/01/2011 12:00
+</t>
   </si>
 </sst>
 </file>
@@ -97,14 +105,15 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="YYYY\-MM\-DD"/>
+    <numFmt numFmtId="164" formatCode="GENERAL"/>
+    <numFmt numFmtId="165" formatCode="DD/MM/YY\ HH:MM"/>
   </numFmts>
   <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -126,6 +135,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -186,12 +196,12 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -218,19 +228,20 @@
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C11" activeCellId="0" sqref="C11"/>
+      <selection pane="topLeft" activeCell="F11" activeCellId="0" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="35.7704081632653"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="39.280612244898"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
@@ -246,7 +257,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
         <v>1</v>
       </c>
@@ -259,111 +270,111 @@
       <c r="D2" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="2" t="n">
-        <v>42552</v>
-      </c>
-      <c r="F2" s="2" t="n">
-        <v>42583</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="n">
         <v>2</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D3" s="0" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="2" t="n">
-        <v>42553</v>
-      </c>
-      <c r="F3" s="3" t="n">
-        <v>42584</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="n">
         <v>3</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4" s="3" t="n">
-        <v>42554</v>
-      </c>
-      <c r="F4" s="3" t="n">
-        <v>42585</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>15</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="n">
         <v>4</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C5" s="0" t="s">
         <v>8</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="E5" s="3" t="n">
-        <v>42555</v>
-      </c>
-      <c r="F5" s="3" t="n">
-        <v>42586</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>14</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="n">
         <v>5</v>
       </c>
       <c r="B6" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="0" t="s">
-        <v>13</v>
-      </c>
       <c r="D6" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="E6" s="3" t="n">
-        <v>42556</v>
-      </c>
-      <c r="F6" s="3" t="n">
-        <v>42587</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>11</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="n">
         <v>6</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="C7" s="0" t="s">
         <v>7</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="E7" s="3" t="n">
-        <v>42557</v>
-      </c>
-      <c r="F7" s="3" t="n">
-        <v>42588</v>
+        <v>22</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>